<commit_message>
Adding report docs and pdf
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uottawa-my.sharepoint.com/personal/ldusa012_uottawa_ca/Documents/2022 Fall/Project dev + mgmt. for cs/GNG-2101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="487" documentId="11_F25DC773A252ABDACC104879A11B6D865ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4BD5BAA-515F-4037-8DC8-030C8376338D}"/>
+  <xr:revisionPtr revIDLastSave="500" documentId="11_F25DC773A252ABDACC104879A11B6D865ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B44BB7EE-DADC-46DE-805E-C0D5B7AF1C1D}"/>
   <bookViews>
-    <workbookView xWindow="11328" yWindow="0" windowWidth="11712" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="528" windowWidth="11712" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="70">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>MB/mintue</t>
+  </si>
+  <si>
+    <t>&gt; 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website or Executable </t>
+  </si>
+  <si>
+    <t>MB/minute</t>
   </si>
 </sst>
 </file>
@@ -377,7 +386,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -432,6 +441,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -720,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F29"/>
+    <sheetView topLeftCell="O26" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1262,16 +1274,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0431FE1-E393-4A5B-AAC5-FC490652822C}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
@@ -1619,7 +1631,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1">
         <v>10</v>
@@ -1632,6 +1644,193 @@
       </c>
       <c r="F18" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>0</v>
+      </c>
+      <c r="B22" s="11">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
+        <v>500</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>6</v>
+      </c>
+      <c r="B27" s="11">
+        <v>4</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
+        <v>2</v>
+      </c>
+      <c r="B28" s="11">
+        <v>1</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
+        <v>5</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
+        <v>100</v>
+      </c>
+      <c r="B37" s="11">
+        <v>10</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>